<commit_message>
Historias de Usuario en pdf
</commit_message>
<xml_diff>
--- a/Historias de Usuario de Coworking.xlsx
+++ b/Historias de Usuario de Coworking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganimedes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programación\Curso MINTIC Fundamentos de programación\Fundamentos de programación\Ciclo 3\G2 Reservas Coworking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E667F6E-C0F8-4C95-BA8E-23464E11E8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBB4C46-4662-4E75-A964-5AB4D58A25F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{9E7F14FF-8562-4637-8C66-C3B8B0D5B460}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E7F14FF-8562-4637-8C66-C3B8B0D5B460}"/>
   </bookViews>
   <sheets>
     <sheet name="Historia de Usuarios" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -399,11 +399,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,6 +433,13 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -431,12 +453,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -455,6 +471,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,417 +815,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE82D5F-780A-4338-BAF3-9FD74A49301E}">
-  <dimension ref="A3:G41"/>
+  <dimension ref="A2:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="D6" sqref="D6:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="55.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="18" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E6" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="3" t="s">
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="3" t="s">
+      <c r="G12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="5" t="s">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="3" t="s">
+      <c r="G16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3" t="s">
+      <c r="G17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5" t="s">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
         <v>1</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="B21" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="D21" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="3" t="s">
+      <c r="G21" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="3" t="s">
+      <c r="G22" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5" t="s">
+      <c r="G23" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
         <v>1</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B26" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="D26" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="3" t="s">
+      <c r="G26" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="3" t="s">
+      <c r="G27" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5" t="s">
+      <c r="G28" s="29"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="29"/>
+    </row>
+    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1190,20 +1237,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
         <v>1</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1213,12 +1260,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="3" t="s">
         <v>12</v>
       </c>
@@ -1226,29 +1273,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1259,20 +1306,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
         <v>1</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="13" t="s">
         <v>53</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1282,40 +1329,40 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
       <c r="F39" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1328,49 +1375,49 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:C40"/>
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="E37:E40"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>